<commit_message>
Add rerun reference dataframes for tests
</commit_message>
<xml_diff>
--- a/data/tests/reference_dataframes/df_cem.xlsx
+++ b/data/tests/reference_dataframes/df_cem.xlsx
@@ -4699,22 +4699,22 @@
         <v>299893.525486403</v>
       </c>
       <c r="H81" t="n">
-        <v>306829.651909123</v>
+        <v>58804.651909123</v>
       </c>
       <c r="I81" t="n">
-        <v>297672.070660933</v>
+        <v>41702.07066093298</v>
       </c>
       <c r="J81" t="n">
-        <v>286606.446940231</v>
+        <v>47068.44694023102</v>
       </c>
       <c r="K81" t="n">
-        <v>295460.746138776</v>
+        <v>39677.74613877601</v>
       </c>
       <c r="L81" t="n">
-        <v>283820.285130871</v>
+        <v>41923.28513087099</v>
       </c>
       <c r="M81" t="n">
-        <v>108527.231495289</v>
+        <v>43351.231495289</v>
       </c>
       <c r="N81" t="n">
         <v>40561.4476921646</v>
@@ -5229,28 +5229,28 @@
         <v>2058956.90203607</v>
       </c>
       <c r="H91" t="n">
-        <v>1981476.17399167</v>
+        <v>401665.1739916699</v>
       </c>
       <c r="I91" t="n">
-        <v>2195403.90927869</v>
+        <v>269367.9092786899</v>
       </c>
       <c r="J91" t="n">
-        <v>2124789.02188846</v>
+        <v>220902.02188846</v>
       </c>
       <c r="K91" t="n">
-        <v>2024382.31793093</v>
+        <v>267272.3179309301</v>
       </c>
       <c r="L91" t="n">
-        <v>2143010.50127022</v>
+        <v>402598.5012702201</v>
       </c>
       <c r="M91" t="n">
-        <v>1966304.75819611</v>
+        <v>429824.7581961099</v>
       </c>
       <c r="N91" t="n">
-        <v>1820053.10059352</v>
+        <v>195590.1005935201</v>
       </c>
       <c r="O91" t="n">
-        <v>1741013.9429687</v>
+        <v>119802.9429687001</v>
       </c>
     </row>
     <row r="92">
@@ -9999,28 +9999,28 @@
         <v>614079.091128438</v>
       </c>
       <c r="H181" t="n">
-        <v>546338.699134178</v>
+        <v>189373.699134178</v>
       </c>
       <c r="I181" t="n">
-        <v>494776.01973774</v>
+        <v>136142.01973774</v>
       </c>
       <c r="J181" t="n">
-        <v>532612.492354495</v>
+        <v>147686.492354495</v>
       </c>
       <c r="K181" t="n">
-        <v>543896.716984358</v>
+        <v>136263.586984358</v>
       </c>
       <c r="L181" t="n">
-        <v>586444.17315306</v>
+        <v>140813.83315306</v>
       </c>
       <c r="M181" t="n">
-        <v>576595.998007861</v>
+        <v>136091.6680078609</v>
       </c>
       <c r="N181" t="n">
-        <v>567399.427902324</v>
+        <v>108306.954902324</v>
       </c>
       <c r="O181" t="n">
-        <v>571141.947070738</v>
+        <v>131967.2200707379</v>
       </c>
     </row>
     <row r="182">

</xml_diff>